<commit_message>
barchart buttons gefixt en initial page gemaakt
</commit_message>
<xml_diff>
--- a/code/data.xlsx
+++ b/code/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Stadsdeel</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>&gt; 681</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
   </si>
 </sst>
 </file>
@@ -187,8 +190,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="127">
+  <cellStyleXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -322,7 +337,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="127">
+  <cellStyles count="139">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -386,6 +401,12 @@
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -449,6 +470,12 @@
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -778,13 +805,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK22"/>
+  <dimension ref="A1:AK24"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="16" max="16" width="26.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" t="s">
@@ -1546,16 +1577,164 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="17" spans="23:37">
+    <row r="9" spans="1:31">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <v>0.32</v>
+      </c>
+      <c r="C9">
+        <v>0.46</v>
+      </c>
+      <c r="D9">
+        <v>0.22</v>
+      </c>
+      <c r="E9">
+        <v>0.41</v>
+      </c>
+      <c r="F9">
+        <v>0.33</v>
+      </c>
+      <c r="G9">
+        <v>0.11</v>
+      </c>
+      <c r="H9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I9">
+        <v>2489</v>
+      </c>
+      <c r="J9">
+        <v>0.32</v>
+      </c>
+      <c r="K9">
+        <v>0.16</v>
+      </c>
+      <c r="L9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M9">
+        <v>0.06</v>
+      </c>
+      <c r="N9">
+        <v>0.09</v>
+      </c>
+      <c r="O9">
+        <v>0.23</v>
+      </c>
+      <c r="P9">
+        <v>0.1</v>
+      </c>
+      <c r="Q9">
+        <v>0.16</v>
+      </c>
+      <c r="R9">
+        <v>0.22</v>
+      </c>
+      <c r="S9">
+        <v>0.35</v>
+      </c>
+      <c r="T9">
+        <v>0.13</v>
+      </c>
+      <c r="U9">
+        <v>0.05</v>
+      </c>
+      <c r="V9">
+        <v>0.06</v>
+      </c>
+      <c r="W9">
+        <v>0.18</v>
+      </c>
+      <c r="X9">
+        <v>0.11</v>
+      </c>
+      <c r="Y9">
+        <v>0.18</v>
+      </c>
+      <c r="Z9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AA9">
+        <v>0.19</v>
+      </c>
+      <c r="AB9">
+        <v>0.03</v>
+      </c>
+      <c r="AC9">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AD9">
+        <v>0.33</v>
+      </c>
+      <c r="AE9">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:31">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:31">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:31">
+      <c r="G13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="Z13" s="1"/>
+    </row>
+    <row r="14" spans="1:31">
+      <c r="G14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="Z14" s="1"/>
+    </row>
+    <row r="15" spans="1:31">
+      <c r="G15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="Z15" s="1"/>
+    </row>
+    <row r="16" spans="1:31">
+      <c r="G16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="Z16" s="1"/>
+    </row>
+    <row r="17" spans="7:37">
+      <c r="G17" s="1"/>
+      <c r="O17" s="1"/>
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
-    <row r="22" spans="23:37">
+    <row r="18" spans="7:37">
+      <c r="G18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="7:37">
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" spans="7:37">
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="7:37">
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="7:37">
+      <c r="S22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
+    </row>
+    <row r="23" spans="7:37">
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="7:37">
+      <c r="S24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
kaart nu per buurt
</commit_message>
<xml_diff>
--- a/code/data.xlsx
+++ b/code/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
   <si>
     <t>Stadsdeel</t>
   </si>
@@ -231,12 +231,6 @@
     <t>F83</t>
   </si>
   <si>
-    <t>F85abc</t>
-  </si>
-  <si>
-    <t>F85defg</t>
-  </si>
-  <si>
     <t>F86</t>
   </si>
   <si>
@@ -451,6 +445,27 @@
   </si>
   <si>
     <t>T94</t>
+  </si>
+  <si>
+    <t>N74</t>
+  </si>
+  <si>
+    <t>F89</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>E75</t>
+  </si>
+  <si>
+    <t>K23</t>
+  </si>
+  <si>
+    <t>M50</t>
   </si>
 </sst>
 </file>
@@ -499,8 +514,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="175">
+  <cellStyleXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -679,7 +716,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="175">
+  <cellStyles count="197">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -767,6 +804,17 @@
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -854,6 +902,17 @@
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1183,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE114"/>
+  <dimension ref="A1:AE119"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="H108" sqref="H108"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1742,7 +1801,7 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B14">
         <v>0.2</v>
@@ -1768,7 +1827,7 @@
     </row>
     <row r="15" spans="1:31">
       <c r="A15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B15">
         <v>0.2</v>
@@ -1794,215 +1853,215 @@
     </row>
     <row r="16" spans="1:31">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="B16">
-        <v>0.34</v>
+        <v>0.2</v>
       </c>
       <c r="C16">
-        <v>0.5</v>
+        <v>0.67</v>
       </c>
       <c r="D16">
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
       <c r="E16">
-        <v>0.56999999999999995</v>
+        <v>0.53</v>
       </c>
       <c r="F16">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="G16">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="H16">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="B17">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="C17">
-        <v>0.43</v>
+        <v>0.67</v>
       </c>
       <c r="D17">
-        <v>0.25</v>
+        <v>0.12</v>
       </c>
       <c r="E17">
-        <v>0.56999999999999995</v>
+        <v>0.53</v>
       </c>
       <c r="F17">
-        <v>0.24</v>
+        <v>0.32</v>
       </c>
       <c r="G17">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="H17">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="B18">
-        <v>0.31</v>
+        <v>0.34</v>
       </c>
       <c r="C18">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
       <c r="D18">
-        <v>0.25</v>
+        <v>0.16</v>
       </c>
       <c r="E18">
         <v>0.56999999999999995</v>
       </c>
       <c r="F18">
-        <v>0.24</v>
+        <v>0.31</v>
       </c>
       <c r="G18">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="H18">
-        <v>0.15</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="B19">
-        <v>0.37</v>
+        <v>0.31</v>
       </c>
       <c r="C19">
-        <v>0.23</v>
+        <v>0.43</v>
       </c>
       <c r="D19">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="E19">
-        <v>0.39</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F19">
-        <v>0.26</v>
+        <v>0.24</v>
       </c>
       <c r="G19">
-        <v>7.0000000000000007E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H19">
-        <v>0.28000000000000003</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="B20">
+        <v>0.31</v>
+      </c>
+      <c r="C20">
+        <v>0.43</v>
+      </c>
+      <c r="D20">
+        <v>0.25</v>
+      </c>
+      <c r="E20">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F20">
         <v>0.24</v>
       </c>
-      <c r="C20">
-        <v>0.4</v>
-      </c>
-      <c r="D20">
-        <v>0.36</v>
-      </c>
-      <c r="E20">
-        <v>0.63</v>
-      </c>
-      <c r="F20">
-        <v>0.21</v>
-      </c>
       <c r="G20">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="H20">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21">
-        <v>0.22</v>
+        <v>0.37</v>
       </c>
       <c r="C21">
-        <v>0.54</v>
+        <v>0.23</v>
       </c>
       <c r="D21">
-        <v>0.24</v>
+        <v>0.4</v>
       </c>
       <c r="E21">
-        <v>0.61</v>
+        <v>0.39</v>
       </c>
       <c r="F21">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="G21">
-        <v>0.02</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H21">
-        <v>0.11</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="B22">
-        <v>0.38</v>
+        <v>0.24</v>
       </c>
       <c r="C22">
-        <v>0.22</v>
+        <v>0.4</v>
       </c>
       <c r="D22">
-        <v>0.39</v>
+        <v>0.36</v>
       </c>
       <c r="E22">
-        <v>0.38</v>
+        <v>0.63</v>
       </c>
       <c r="F22">
-        <v>0.28000000000000003</v>
+        <v>0.21</v>
       </c>
       <c r="G22">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="H22">
-        <v>0.22</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="C23">
-        <v>0.2</v>
+        <v>0.54</v>
       </c>
       <c r="D23">
-        <v>0.4</v>
+        <v>0.24</v>
       </c>
       <c r="E23">
-        <v>0.52</v>
+        <v>0.61</v>
       </c>
       <c r="F23">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="G23">
         <v>0.02</v>
       </c>
       <c r="H23">
-        <v>0.21</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B24">
         <v>0.38</v>
@@ -2028,66 +2087,59 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="B25">
-        <v>0.18</v>
+        <v>0.4</v>
       </c>
       <c r="C25">
-        <v>0.54</v>
+        <v>0.2</v>
       </c>
       <c r="D25">
-        <v>0.28999999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="E25">
-        <v>0.6</v>
+        <v>0.52</v>
       </c>
       <c r="F25">
-        <v>0.23</v>
+        <v>0.26</v>
       </c>
       <c r="G25">
-        <v>0.12</v>
+        <v>0.02</v>
       </c>
       <c r="H25">
-        <v>0.04</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="B26">
-        <f>AVERAGE(B27:B29)</f>
-        <v>0.24333333333333332</v>
+        <v>0.38</v>
       </c>
       <c r="C26">
-        <f>AVERAGE(C27:C29)</f>
-        <v>0.5033333333333333</v>
+        <v>0.22</v>
       </c>
       <c r="D26">
-        <f>AVERAGE(D27:D29)</f>
-        <v>0.25666666666666665</v>
+        <v>0.39</v>
       </c>
       <c r="E26">
-        <f>AVERAGE(E27:E29)</f>
-        <v>0.56666666666666676</v>
+        <v>0.38</v>
       </c>
       <c r="F26">
-        <f>AVERAGE(F27:F29)</f>
-        <v>0.26333333333333336</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G26">
-        <f>AVERAGE(G27:G29)</f>
-        <v>0.10000000000000002</v>
+        <v>0.13</v>
       </c>
       <c r="H26">
-        <f>AVERAGE(H27:H29)</f>
-        <v>6.3333333333333339E-2</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>113</v>
       </c>
       <c r="B27">
         <v>0.18</v>
@@ -2113,423 +2165,454 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>133</v>
       </c>
       <c r="B28">
-        <v>0.26</v>
+        <f>AVERAGE(B29:B31)</f>
+        <v>0.24333333333333332</v>
       </c>
       <c r="C28">
-        <v>0.52</v>
+        <f>AVERAGE(C29:C31)</f>
+        <v>0.5033333333333333</v>
       </c>
       <c r="D28">
-        <v>0.22</v>
+        <f>AVERAGE(D29:D31)</f>
+        <v>0.25666666666666665</v>
       </c>
       <c r="E28">
-        <v>0.54</v>
+        <f>AVERAGE(E29:E31)</f>
+        <v>0.56666666666666676</v>
       </c>
       <c r="F28">
-        <v>0.31</v>
+        <f>AVERAGE(F29:F31)</f>
+        <v>0.26333333333333336</v>
       </c>
       <c r="G28">
-        <v>0.08</v>
+        <f>AVERAGE(G29:G31)</f>
+        <v>0.10000000000000002</v>
       </c>
       <c r="H28">
-        <v>0.06</v>
+        <f>AVERAGE(H29:H31)</f>
+        <v>6.3333333333333339E-2</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29">
+        <v>0.18</v>
+      </c>
+      <c r="C29">
+        <v>0.54</v>
+      </c>
+      <c r="D29">
         <v>0.28999999999999998</v>
       </c>
-      <c r="C29">
-        <v>0.45</v>
-      </c>
-      <c r="D29">
-        <v>0.26</v>
-      </c>
       <c r="E29">
-        <v>0.56000000000000005</v>
+        <v>0.6</v>
       </c>
       <c r="F29">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="G29">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="H29">
-        <v>0.09</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B30">
-        <v>0.46</v>
+        <v>0.26</v>
       </c>
       <c r="C30">
-        <v>0.19</v>
+        <v>0.52</v>
       </c>
       <c r="D30">
-        <v>0.35</v>
+        <v>0.22</v>
       </c>
       <c r="E30">
-        <v>0.48</v>
+        <v>0.54</v>
       </c>
       <c r="F30">
-        <v>0.36</v>
+        <v>0.31</v>
       </c>
       <c r="G30">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
       <c r="H30">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31">
-        <v>0.18</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C31">
-        <v>0.74</v>
+        <v>0.45</v>
       </c>
       <c r="D31">
-        <v>0.08</v>
+        <v>0.26</v>
       </c>
       <c r="E31">
-        <v>0.62</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F31">
-        <v>0.16</v>
+        <v>0.25</v>
       </c>
       <c r="G31">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="H31">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="B32">
-        <f xml:space="preserve"> AVERAGE(B33:B34)</f>
-        <v>0.315</v>
+        <v>0.46</v>
+      </c>
+      <c r="C32">
+        <v>0.19</v>
+      </c>
+      <c r="D32">
+        <v>0.35</v>
+      </c>
+      <c r="E32">
+        <v>0.48</v>
+      </c>
+      <c r="F32">
+        <v>0.36</v>
+      </c>
+      <c r="G32">
+        <v>0.15</v>
+      </c>
+      <c r="H32">
+        <v>0.02</v>
       </c>
     </row>
     <row r="33" spans="1:31">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33">
-        <v>0.37</v>
+        <v>0.18</v>
       </c>
       <c r="C33">
-        <v>0.21</v>
+        <v>0.74</v>
       </c>
       <c r="D33">
-        <v>0.42</v>
+        <v>0.08</v>
       </c>
       <c r="E33">
-        <v>0.56999999999999995</v>
+        <v>0.62</v>
       </c>
       <c r="F33">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="G33">
+        <v>0.13</v>
+      </c>
+      <c r="H33">
         <v>0.08</v>
-      </c>
-      <c r="H33">
-        <v>0.15</v>
       </c>
     </row>
     <row r="34" spans="1:31">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
       <c r="B34">
-        <v>0.26</v>
+        <f xml:space="preserve"> AVERAGE(B35:B36)</f>
+        <v>0.315</v>
       </c>
       <c r="C34">
-        <v>0.45</v>
+        <f>AVERAGE(C35:C36)</f>
+        <v>0.33</v>
       </c>
       <c r="D34">
-        <v>0.28999999999999998</v>
+        <f>AVERAGE(D35:D36)</f>
+        <v>0.35499999999999998</v>
       </c>
       <c r="E34">
-        <v>0.53</v>
+        <f>AVERAGE(E35:E36)</f>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F34">
-        <v>0.35</v>
+        <f>AVERAGE(F35:F36)</f>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G34">
-        <v>0.06</v>
+        <f>AVERAGE(G35:G36)</f>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H34">
-        <v>7.0000000000000007E-2</v>
+        <f>AVERAGE(H35:H36)</f>
+        <v>0.11</v>
       </c>
     </row>
     <row r="35" spans="1:31">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B35">
-        <v>0.23</v>
+        <v>0.37</v>
       </c>
       <c r="C35">
-        <v>0.51</v>
+        <v>0.21</v>
       </c>
       <c r="D35">
-        <v>0.26</v>
+        <v>0.42</v>
       </c>
       <c r="E35">
-        <v>0.6</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F35">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="G35">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H35">
-        <v>7.0000000000000007E-2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="36" spans="1:31">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36">
-        <v>0.24</v>
+        <v>0.26</v>
       </c>
       <c r="C36">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="D36">
-        <v>0.33</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E36">
-        <v>0.61</v>
+        <v>0.53</v>
       </c>
       <c r="F36">
-        <v>0.28999999999999998</v>
+        <v>0.35</v>
       </c>
       <c r="G36">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="H36">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="37" spans="1:31">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37">
-        <v>0.31</v>
+        <v>0.23</v>
       </c>
       <c r="C37">
-        <v>0.21</v>
+        <v>0.51</v>
       </c>
       <c r="D37">
-        <v>0.48</v>
+        <v>0.26</v>
       </c>
       <c r="E37">
-        <v>0.33</v>
+        <v>0.6</v>
       </c>
       <c r="F37">
-        <v>0.4</v>
+        <v>0.23</v>
       </c>
       <c r="G37">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="H37">
-        <v>0.14000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="38" spans="1:31">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B38">
-        <v>0.32</v>
+        <v>0.24</v>
       </c>
       <c r="C38">
-        <v>0.55000000000000004</v>
+        <v>0.43</v>
       </c>
       <c r="D38">
-        <v>0.13</v>
+        <v>0.33</v>
       </c>
       <c r="E38">
-        <v>0.36</v>
+        <v>0.61</v>
       </c>
       <c r="F38">
-        <v>0.36</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="G38">
-        <v>0.14000000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="H38">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I38">
-        <v>2312</v>
-      </c>
-      <c r="J38">
-        <v>0.31</v>
-      </c>
-      <c r="K38">
-        <v>0.17</v>
-      </c>
-      <c r="L38">
-        <v>0.17</v>
-      </c>
-      <c r="M38">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N38">
-        <v>0.1</v>
-      </c>
-      <c r="O38">
-        <v>0.17</v>
-      </c>
-      <c r="P38">
-        <v>0.03</v>
-      </c>
-      <c r="Q38">
-        <v>0.16</v>
-      </c>
-      <c r="R38">
-        <v>0.15</v>
-      </c>
-      <c r="S38">
-        <v>0.49</v>
-      </c>
-      <c r="T38">
-        <v>0.13</v>
-      </c>
-      <c r="U38">
-        <v>0.04</v>
-      </c>
-      <c r="V38">
-        <v>0.02</v>
-      </c>
-      <c r="W38">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="X38">
-        <v>0.1</v>
-      </c>
-      <c r="Y38">
-        <v>0.2</v>
-      </c>
-      <c r="Z38">
-        <v>0.3</v>
-      </c>
-      <c r="AA38">
-        <v>0.25</v>
-      </c>
-      <c r="AB38">
-        <v>0.02</v>
-      </c>
-      <c r="AC38">
-        <v>0.43</v>
-      </c>
-      <c r="AD38">
-        <v>0.37</v>
-      </c>
-      <c r="AE38">
-        <v>0.18</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="39" spans="1:31">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="B39">
-        <v>0.22</v>
+        <v>0.31</v>
       </c>
       <c r="C39">
-        <v>0.7</v>
+        <v>0.21</v>
       </c>
       <c r="D39">
-        <v>0.08</v>
+        <v>0.48</v>
       </c>
       <c r="E39">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="F39">
-        <v>0.32</v>
+        <v>0.4</v>
       </c>
       <c r="G39">
-        <v>0.21</v>
+        <v>0.13</v>
       </c>
       <c r="H39">
-        <v>0.12</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:31">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="B40">
-        <v>0.28000000000000003</v>
+        <v>0.315</v>
       </c>
       <c r="C40">
-        <v>0.67</v>
+        <v>0.33</v>
       </c>
       <c r="D40">
-        <v>0.05</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="E40">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F40">
-        <v>0.31</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G40">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H40">
-        <v>0.02</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="41" spans="1:31">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="B41">
-        <v>0.24</v>
+        <v>0.32</v>
       </c>
       <c r="C41">
-        <v>0.72</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D41">
+        <v>0.13</v>
+      </c>
+      <c r="E41">
+        <v>0.36</v>
+      </c>
+      <c r="F41">
+        <v>0.36</v>
+      </c>
+      <c r="G41">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H41">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I41">
+        <v>2312</v>
+      </c>
+      <c r="J41">
+        <v>0.31</v>
+      </c>
+      <c r="K41">
+        <v>0.17</v>
+      </c>
+      <c r="L41">
+        <v>0.17</v>
+      </c>
+      <c r="M41">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N41">
+        <v>0.1</v>
+      </c>
+      <c r="O41">
+        <v>0.17</v>
+      </c>
+      <c r="P41">
+        <v>0.03</v>
+      </c>
+      <c r="Q41">
+        <v>0.16</v>
+      </c>
+      <c r="R41">
+        <v>0.15</v>
+      </c>
+      <c r="S41">
+        <v>0.49</v>
+      </c>
+      <c r="T41">
+        <v>0.13</v>
+      </c>
+      <c r="U41">
         <v>0.04</v>
       </c>
-      <c r="E41">
-        <v>0.62</v>
-      </c>
-      <c r="F41">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="G41">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="H41">
+      <c r="V41">
         <v>0.02</v>
+      </c>
+      <c r="W41">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="X41">
+        <v>0.1</v>
+      </c>
+      <c r="Y41">
+        <v>0.2</v>
+      </c>
+      <c r="Z41">
+        <v>0.3</v>
+      </c>
+      <c r="AA41">
+        <v>0.25</v>
+      </c>
+      <c r="AB41">
+        <v>0.02</v>
+      </c>
+      <c r="AC41">
+        <v>0.43</v>
+      </c>
+      <c r="AD41">
+        <v>0.37</v>
+      </c>
+      <c r="AE41">
+        <v>0.18</v>
       </c>
     </row>
     <row r="42" spans="1:31">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B42">
         <v>0.22</v>
@@ -2555,214 +2638,207 @@
     </row>
     <row r="43" spans="1:31">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B43">
-        <v>0.48</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C43">
-        <v>0.52</v>
+        <v>0.67</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="F43">
-        <v>0.23</v>
+        <v>0.31</v>
       </c>
       <c r="G43">
-        <v>0.4</v>
+        <v>0.06</v>
       </c>
       <c r="H43">
-        <v>0.37</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="44" spans="1:31">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="B44">
-        <v>0.57999999999999996</v>
+        <v>0.24</v>
       </c>
       <c r="C44">
+        <v>0.72</v>
+      </c>
+      <c r="D44">
+        <v>0.04</v>
+      </c>
+      <c r="E44">
+        <v>0.62</v>
+      </c>
+      <c r="F44">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D44">
-        <v>0.13</v>
-      </c>
-      <c r="E44">
-        <v>0.21</v>
-      </c>
-      <c r="F44">
-        <v>0.33</v>
-      </c>
       <c r="G44">
-        <v>0.25</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H44">
-        <v>0.21</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="45" spans="1:31">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>136</v>
       </c>
       <c r="B45">
-        <v>0.27</v>
+        <v>0.22</v>
       </c>
       <c r="C45">
-        <v>0.63</v>
+        <v>0.7</v>
       </c>
       <c r="D45">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="E45">
-        <v>0.48</v>
+        <v>0.35</v>
       </c>
       <c r="F45">
-        <v>0.43</v>
+        <v>0.32</v>
       </c>
       <c r="G45">
-        <v>7.0000000000000007E-2</v>
+        <v>0.21</v>
       </c>
       <c r="H45">
-        <v>0.02</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="46" spans="1:31">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B46">
-        <v>0.31</v>
+        <v>0.48</v>
       </c>
       <c r="C46">
-        <v>0.62</v>
+        <v>0.52</v>
       </c>
       <c r="D46">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
         <v>0.23</v>
       </c>
-      <c r="F46">
-        <v>0.47</v>
-      </c>
       <c r="G46">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="H46">
-        <v>0.15</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="47" spans="1:31">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="B47">
-        <v>0.45</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="C47">
-        <v>0.52</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D47">
-        <v>0.04</v>
+        <v>0.13</v>
       </c>
       <c r="E47">
-        <v>0.45</v>
+        <v>0.21</v>
       </c>
       <c r="F47">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G47">
-        <v>0.08</v>
+        <v>0.25</v>
       </c>
       <c r="H47">
-        <v>7.0000000000000007E-2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="48" spans="1:31">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="B48">
-        <v>0.57999999999999996</v>
+        <v>0.27</v>
       </c>
       <c r="C48">
-        <v>0.28999999999999998</v>
+        <v>0.63</v>
       </c>
       <c r="D48">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="E48">
-        <v>0.21</v>
+        <v>0.48</v>
       </c>
       <c r="F48">
-        <v>0.33</v>
+        <v>0.43</v>
       </c>
       <c r="G48">
-        <v>0.25</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H48">
-        <v>0.21</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="49" spans="1:31">
       <c r="A49" t="s">
-        <v>141</v>
+        <v>68</v>
       </c>
       <c r="B49">
-        <f>AVERAGE(B50:B51)</f>
-        <v>0.27999999999999997</v>
+        <v>0.31</v>
       </c>
       <c r="C49">
-        <f>AVERAGE(C50:C51)</f>
-        <v>0.56999999999999995</v>
+        <v>0.62</v>
       </c>
       <c r="D49">
-        <f>AVERAGE(D50:D51)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E49">
+        <v>0.23</v>
+      </c>
+      <c r="F49">
+        <v>0.47</v>
+      </c>
+      <c r="G49">
         <v>0.15</v>
       </c>
-      <c r="E49">
-        <f>AVERAGE(E50:E51)</f>
-        <v>0.25</v>
-      </c>
-      <c r="F49">
-        <f>AVERAGE(F50:F51)</f>
-        <v>0.48</v>
-      </c>
-      <c r="G49">
-        <f>AVERAGE(G50:G51)</f>
-        <v>0.17499999999999999</v>
-      </c>
       <c r="H49">
-        <f>AVERAGE(H50:H51)</f>
-        <v>8.5000000000000006E-2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="50" spans="1:31">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B50">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="C50">
-        <v>0.44</v>
+        <v>0.52</v>
       </c>
       <c r="D50">
-        <v>0.21</v>
+        <v>0.04</v>
       </c>
       <c r="E50">
-        <v>0.28000000000000003</v>
+        <v>0.45</v>
       </c>
       <c r="F50">
-        <v>0.48</v>
+        <v>0.4</v>
       </c>
       <c r="G50">
-        <v>0.16</v>
+        <v>0.08</v>
       </c>
       <c r="H50">
         <v>7.0000000000000007E-2</v>
@@ -2770,839 +2846,839 @@
     </row>
     <row r="51" spans="1:31">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="B51">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C51">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D51">
+        <v>0.13</v>
+      </c>
+      <c r="E51">
         <v>0.21</v>
       </c>
-      <c r="C51">
-        <v>0.7</v>
-      </c>
-      <c r="D51">
-        <v>0.09</v>
-      </c>
-      <c r="E51">
-        <v>0.22</v>
-      </c>
       <c r="F51">
-        <v>0.48</v>
+        <v>0.33</v>
       </c>
       <c r="G51">
-        <v>0.19</v>
+        <v>0.25</v>
       </c>
       <c r="H51">
-        <v>0.1</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="52" spans="1:31">
       <c r="A52" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="B52">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="C52">
-        <v>0.53</v>
+        <v>0.44</v>
       </c>
       <c r="D52">
-        <v>0.28000000000000003</v>
+        <v>0.21</v>
       </c>
       <c r="E52">
         <v>0.28000000000000003</v>
       </c>
       <c r="F52">
-        <v>0.28999999999999998</v>
+        <v>0.48</v>
       </c>
       <c r="G52">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="H52">
-        <v>0.28999999999999998</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="53" spans="1:31">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="B53">
+        <v>0.35</v>
+      </c>
+      <c r="C53">
+        <v>0.44</v>
+      </c>
+      <c r="D53">
+        <v>0.21</v>
+      </c>
+      <c r="E53">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C53">
-        <v>0.46</v>
-      </c>
-      <c r="D53">
-        <v>0.26</v>
-      </c>
-      <c r="E53">
-        <v>0.28999999999999998</v>
-      </c>
       <c r="F53">
-        <v>0.35</v>
+        <v>0.48</v>
       </c>
       <c r="G53">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="H53">
-        <v>0.21</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="54" spans="1:31">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B54">
-        <v>0.51</v>
+        <v>0.2</v>
       </c>
       <c r="C54">
-        <v>0.21</v>
+        <v>0.53</v>
       </c>
       <c r="D54">
         <v>0.28000000000000003</v>
       </c>
       <c r="E54">
-        <v>0.01</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F54">
-        <v>0.24</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="G54">
-        <v>0.23</v>
+        <v>0.13</v>
       </c>
       <c r="H54">
-        <v>0.52</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:31">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="B55">
-        <v>0.32</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C55">
-        <v>0.3</v>
+        <v>0.46</v>
       </c>
       <c r="D55">
-        <v>0.38</v>
+        <v>0.26</v>
       </c>
       <c r="E55">
-        <v>0.41</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F55">
-        <v>0.28000000000000003</v>
+        <v>0.35</v>
       </c>
       <c r="G55">
-        <v>0.11</v>
+        <v>0.15</v>
       </c>
       <c r="H55">
         <v>0.21</v>
       </c>
-      <c r="I55">
-        <v>2887</v>
-      </c>
-      <c r="J55">
-        <v>0.26</v>
-      </c>
-      <c r="K55">
-        <v>0.16</v>
-      </c>
-      <c r="L55">
-        <v>0.13</v>
-      </c>
-      <c r="M55">
-        <v>0.05</v>
-      </c>
-      <c r="N55">
-        <v>0.11</v>
-      </c>
-      <c r="O55">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="P55">
-        <v>0.11</v>
-      </c>
-      <c r="Q55">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="R55">
-        <v>0.31</v>
-      </c>
-      <c r="S55">
-        <v>0.24</v>
-      </c>
-      <c r="T55">
-        <v>0.16</v>
-      </c>
-      <c r="U55">
-        <v>0.04</v>
-      </c>
-      <c r="V55">
-        <v>0.03</v>
-      </c>
-      <c r="W55">
-        <v>0.16</v>
-      </c>
-      <c r="X55">
-        <v>0.11</v>
-      </c>
-      <c r="Y55">
-        <v>0.15</v>
-      </c>
-      <c r="Z55">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="AA55">
-        <v>0.25</v>
-      </c>
-      <c r="AB55">
-        <v>0.02</v>
-      </c>
-      <c r="AC55">
-        <v>0.22</v>
-      </c>
-      <c r="AD55">
-        <v>0.31</v>
-      </c>
-      <c r="AE55">
-        <v>0.45</v>
-      </c>
     </row>
     <row r="56" spans="1:31">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B56">
-        <v>0.27</v>
+        <v>0.51</v>
       </c>
       <c r="C56">
+        <v>0.21</v>
+      </c>
+      <c r="D56">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D56">
-        <v>0.45</v>
-      </c>
       <c r="E56">
-        <v>0.55000000000000004</v>
+        <v>0.01</v>
       </c>
       <c r="F56">
         <v>0.24</v>
       </c>
       <c r="G56">
-        <v>0.08</v>
+        <v>0.23</v>
       </c>
       <c r="H56">
-        <v>0.13</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="57" spans="1:31">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="B57">
-        <v>0.34</v>
+        <v>0.32</v>
       </c>
       <c r="C57">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="D57">
-        <v>0.33</v>
+        <v>0.38</v>
       </c>
       <c r="E57">
-        <v>0.61</v>
+        <v>0.41</v>
       </c>
       <c r="F57">
-        <v>0.23</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G57">
+        <v>0.11</v>
+      </c>
+      <c r="H57">
+        <v>0.21</v>
+      </c>
+      <c r="I57">
+        <v>2887</v>
+      </c>
+      <c r="J57">
+        <v>0.26</v>
+      </c>
+      <c r="K57">
+        <v>0.16</v>
+      </c>
+      <c r="L57">
+        <v>0.13</v>
+      </c>
+      <c r="M57">
         <v>0.05</v>
       </c>
-      <c r="H57">
+      <c r="N57">
         <v>0.11</v>
+      </c>
+      <c r="O57">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="P57">
+        <v>0.11</v>
+      </c>
+      <c r="Q57">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R57">
+        <v>0.31</v>
+      </c>
+      <c r="S57">
+        <v>0.24</v>
+      </c>
+      <c r="T57">
+        <v>0.16</v>
+      </c>
+      <c r="U57">
+        <v>0.04</v>
+      </c>
+      <c r="V57">
+        <v>0.03</v>
+      </c>
+      <c r="W57">
+        <v>0.16</v>
+      </c>
+      <c r="X57">
+        <v>0.11</v>
+      </c>
+      <c r="Y57">
+        <v>0.15</v>
+      </c>
+      <c r="Z57">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AA57">
+        <v>0.25</v>
+      </c>
+      <c r="AB57">
+        <v>0.02</v>
+      </c>
+      <c r="AC57">
+        <v>0.22</v>
+      </c>
+      <c r="AD57">
+        <v>0.31</v>
+      </c>
+      <c r="AE57">
+        <v>0.45</v>
       </c>
     </row>
     <row r="58" spans="1:31">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="B58">
-        <v>0.16</v>
+        <v>0.45</v>
       </c>
       <c r="C58">
-        <v>0.76</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D58">
-        <v>0.09</v>
+        <v>0.27</v>
       </c>
       <c r="E58">
-        <v>0.56999999999999995</v>
+        <v>0.3</v>
       </c>
       <c r="F58">
-        <v>0.33</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G58">
-        <v>0.06</v>
+        <v>0.24</v>
       </c>
       <c r="H58">
-        <v>0.04</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="59" spans="1:31">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B59">
-        <v>0.39</v>
+        <v>0.27</v>
       </c>
       <c r="C59">
-        <v>0.15</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D59">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
       <c r="E59">
-        <v>0.46</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F59">
-        <v>0.33</v>
+        <v>0.24</v>
       </c>
       <c r="G59">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="H59">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="60" spans="1:31">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B60">
         <v>0.34</v>
       </c>
       <c r="C60">
-        <v>0.35</v>
+        <v>0.32</v>
       </c>
       <c r="D60">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
       <c r="E60">
-        <v>0.59</v>
+        <v>0.61</v>
       </c>
       <c r="F60">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
       <c r="G60">
+        <v>0.05</v>
+      </c>
+      <c r="H60">
         <v>0.11</v>
-      </c>
-      <c r="H60">
-        <v>0.09</v>
       </c>
     </row>
     <row r="61" spans="1:31">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B61">
-        <v>0.47</v>
+        <v>0.16</v>
       </c>
       <c r="C61">
-        <v>0.1</v>
+        <v>0.76</v>
       </c>
       <c r="D61">
-        <v>0.43</v>
+        <v>0.09</v>
       </c>
       <c r="E61">
-        <v>0.18</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F61">
-        <v>0.18</v>
+        <v>0.33</v>
       </c>
       <c r="G61">
-        <v>0.13</v>
+        <v>0.06</v>
       </c>
       <c r="H61">
-        <v>0.52</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="62" spans="1:31">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="B62">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="C62">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="D62">
-        <v>0.59</v>
+        <v>0.46</v>
       </c>
       <c r="E62">
-        <v>0.3</v>
+        <v>0.46</v>
       </c>
       <c r="F62">
-        <v>0.21</v>
+        <v>0.33</v>
       </c>
       <c r="G62">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="H62">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="63" spans="1:31">
       <c r="A63" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B63">
-        <v>0.14000000000000001</v>
+        <v>0.34</v>
       </c>
       <c r="C63">
-        <v>0.55000000000000004</v>
+        <v>0.35</v>
       </c>
       <c r="D63">
         <v>0.31</v>
       </c>
       <c r="E63">
-        <v>0.39</v>
+        <v>0.59</v>
       </c>
       <c r="F63">
-        <v>0.36</v>
+        <v>0.21</v>
       </c>
       <c r="G63">
+        <v>0.11</v>
+      </c>
+      <c r="H63">
         <v>0.09</v>
-      </c>
-      <c r="H63">
-        <v>0.17</v>
       </c>
     </row>
     <row r="64" spans="1:31">
       <c r="A64" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="B64">
-        <v>0.37</v>
+        <v>0.47</v>
       </c>
       <c r="C64">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="D64">
-        <v>0.59</v>
+        <v>0.43</v>
       </c>
       <c r="E64">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="F64">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
       <c r="G64">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="H64">
-        <v>0.4</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="65" spans="1:31">
       <c r="A65" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="B65">
-        <v>0.6</v>
+        <v>0.37</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D65">
+        <v>0.59</v>
+      </c>
+      <c r="E65">
+        <v>0.3</v>
+      </c>
+      <c r="F65">
+        <v>0.21</v>
+      </c>
+      <c r="G65">
+        <v>0.1</v>
+      </c>
+      <c r="H65">
         <v>0.4</v>
-      </c>
-      <c r="E65">
-        <v>0.05</v>
-      </c>
-      <c r="F65">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G65">
-        <v>0.09</v>
-      </c>
-      <c r="H65">
-        <v>0.79</v>
       </c>
     </row>
     <row r="66" spans="1:31">
       <c r="A66" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B66">
-        <v>0.26</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C66">
-        <v>0.19</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D66">
-        <v>0.55000000000000004</v>
+        <v>0.31</v>
       </c>
       <c r="E66">
-        <v>0.24</v>
+        <v>0.39</v>
       </c>
       <c r="F66">
-        <v>0.33</v>
+        <v>0.36</v>
       </c>
       <c r="G66">
-        <v>0.14000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="H66">
-        <v>0.28999999999999998</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="67" spans="1:31">
       <c r="A67" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="B67">
-        <v>0.2</v>
+        <v>0.37</v>
       </c>
       <c r="C67">
-        <v>0.46</v>
+        <v>0.05</v>
       </c>
       <c r="D67">
-        <v>0.34</v>
+        <v>0.59</v>
       </c>
       <c r="E67">
-        <v>0.37</v>
+        <v>0.3</v>
       </c>
       <c r="F67">
-        <v>0.31</v>
+        <v>0.21</v>
       </c>
       <c r="G67">
-        <v>0.14000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="H67">
-        <v>0.17</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="68" spans="1:31">
       <c r="A68" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B68">
-        <v>0.19</v>
+        <v>0.6</v>
       </c>
       <c r="C68">
-        <v>0.43</v>
+        <v>0</v>
       </c>
       <c r="D68">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="E68">
-        <v>0.44</v>
+        <v>0.05</v>
       </c>
       <c r="F68">
-        <v>0.34</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G68">
         <v>0.09</v>
       </c>
       <c r="H68">
-        <v>0.13</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="69" spans="1:31">
       <c r="A69" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="B69">
-        <v>0.45</v>
+        <v>0.26</v>
       </c>
       <c r="C69">
-        <v>0.28000000000000003</v>
+        <v>0.19</v>
       </c>
       <c r="D69">
-        <v>0.27</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E69">
-        <v>0.3</v>
+        <v>0.24</v>
       </c>
       <c r="F69">
-        <v>0.28000000000000003</v>
+        <v>0.33</v>
       </c>
       <c r="G69">
-        <v>0.24</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H69">
-        <v>0.19</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="70" spans="1:31">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B70">
-        <v>0.41</v>
+        <v>0.2</v>
       </c>
       <c r="C70">
-        <v>0.32</v>
+        <v>0.46</v>
       </c>
       <c r="D70">
-        <v>0.28000000000000003</v>
+        <v>0.34</v>
       </c>
       <c r="E70">
-        <v>0.28000000000000003</v>
+        <v>0.37</v>
       </c>
       <c r="F70">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="G70">
-        <v>0.1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H70">
-        <v>0.32</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="71" spans="1:31">
       <c r="A71" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
       <c r="B71">
-        <v>0.45</v>
+        <v>0.19</v>
       </c>
       <c r="C71">
-        <v>0.28000000000000003</v>
+        <v>0.43</v>
       </c>
       <c r="D71">
-        <v>0.27</v>
+        <v>0.38</v>
       </c>
       <c r="E71">
-        <v>0.3</v>
+        <v>0.44</v>
       </c>
       <c r="F71">
-        <v>0.28000000000000003</v>
+        <v>0.34</v>
       </c>
       <c r="G71">
-        <v>0.24</v>
+        <v>0.09</v>
       </c>
       <c r="H71">
-        <v>0.19</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="72" spans="1:31">
       <c r="A72" t="s">
-        <v>5</v>
+        <v>118</v>
       </c>
       <c r="B72">
-        <v>0.32</v>
+        <v>0.45</v>
       </c>
       <c r="C72">
-        <v>0.51</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D72">
-        <v>0.17</v>
+        <v>0.27</v>
       </c>
       <c r="E72">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="F72">
-        <v>0.35</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G72">
-        <v>0.1</v>
+        <v>0.24</v>
       </c>
       <c r="H72">
-        <v>0.15</v>
-      </c>
-      <c r="I72">
-        <v>2596</v>
-      </c>
-      <c r="J72">
-        <v>0.3</v>
-      </c>
-      <c r="K72">
-        <v>0.15</v>
-      </c>
-      <c r="L72">
-        <v>0.15</v>
-      </c>
-      <c r="M72">
-        <v>0.05</v>
-      </c>
-      <c r="N72">
-        <v>0.08</v>
-      </c>
-      <c r="O72">
-        <v>0.27</v>
-      </c>
-      <c r="P72">
-        <v>0.09</v>
-      </c>
-      <c r="Q72">
-        <v>0.13</v>
-      </c>
-      <c r="R72">
-        <v>0.21</v>
-      </c>
-      <c r="S72">
-        <v>0.4</v>
-      </c>
-      <c r="T72">
-        <v>0.13</v>
-      </c>
-      <c r="U72">
-        <v>0.05</v>
-      </c>
-      <c r="V72">
-        <v>0.04</v>
-      </c>
-      <c r="W72">
-        <v>0.15</v>
-      </c>
-      <c r="X72">
-        <v>0.12</v>
-      </c>
-      <c r="Y72">
-        <v>0.22</v>
-      </c>
-      <c r="Z72">
-        <v>0.3</v>
-      </c>
-      <c r="AA72">
-        <v>0.17</v>
-      </c>
-      <c r="AB72">
-        <v>0.02</v>
-      </c>
-      <c r="AC72">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="AD72">
-        <v>0.31</v>
-      </c>
-      <c r="AE72">
-        <v>0.38</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="73" spans="1:31">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B73">
-        <v>0.44</v>
+        <v>0.41</v>
       </c>
       <c r="C73">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="D73">
-        <v>0.26</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E73">
-        <v>0.61</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F73">
-        <v>0.19</v>
+        <v>0.3</v>
       </c>
       <c r="G73">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="H73">
-        <v>0.12</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="74" spans="1:31">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
       <c r="B74">
+        <v>0.45</v>
+      </c>
+      <c r="C74">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D74">
+        <v>0.27</v>
+      </c>
+      <c r="E74">
+        <v>0.3</v>
+      </c>
+      <c r="F74">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G74">
         <v>0.24</v>
       </c>
-      <c r="C74">
-        <v>0.6</v>
-      </c>
-      <c r="D74">
-        <v>0.15</v>
-      </c>
-      <c r="E74">
-        <v>0.48</v>
-      </c>
-      <c r="F74">
-        <v>0.35</v>
-      </c>
-      <c r="G74">
-        <v>7.0000000000000007E-2</v>
-      </c>
       <c r="H74">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="75" spans="1:31">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="B75">
+        <v>0.32</v>
+      </c>
+      <c r="C75">
+        <v>0.51</v>
+      </c>
+      <c r="D75">
+        <v>0.17</v>
+      </c>
+      <c r="E75">
+        <v>0.4</v>
+      </c>
+      <c r="F75">
+        <v>0.35</v>
+      </c>
+      <c r="G75">
+        <v>0.1</v>
+      </c>
+      <c r="H75">
+        <v>0.15</v>
+      </c>
+      <c r="I75">
+        <v>2596</v>
+      </c>
+      <c r="J75">
+        <v>0.3</v>
+      </c>
+      <c r="K75">
+        <v>0.15</v>
+      </c>
+      <c r="L75">
+        <v>0.15</v>
+      </c>
+      <c r="M75">
+        <v>0.05</v>
+      </c>
+      <c r="N75">
+        <v>0.08</v>
+      </c>
+      <c r="O75">
+        <v>0.27</v>
+      </c>
+      <c r="P75">
+        <v>0.09</v>
+      </c>
+      <c r="Q75">
+        <v>0.13</v>
+      </c>
+      <c r="R75">
+        <v>0.21</v>
+      </c>
+      <c r="S75">
+        <v>0.4</v>
+      </c>
+      <c r="T75">
+        <v>0.13</v>
+      </c>
+      <c r="U75">
+        <v>0.05</v>
+      </c>
+      <c r="V75">
+        <v>0.04</v>
+      </c>
+      <c r="W75">
+        <v>0.15</v>
+      </c>
+      <c r="X75">
+        <v>0.12</v>
+      </c>
+      <c r="Y75">
         <v>0.22</v>
       </c>
-      <c r="C75">
-        <v>0.66</v>
-      </c>
-      <c r="D75">
-        <v>0.12</v>
-      </c>
-      <c r="E75">
-        <v>0.43</v>
-      </c>
-      <c r="F75">
-        <v>0.42</v>
-      </c>
-      <c r="G75">
-        <v>0.04</v>
-      </c>
-      <c r="H75">
-        <v>0.1</v>
+      <c r="Z75">
+        <v>0.3</v>
+      </c>
+      <c r="AA75">
+        <v>0.17</v>
+      </c>
+      <c r="AB75">
+        <v>0.02</v>
+      </c>
+      <c r="AC75">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AD75">
+        <v>0.31</v>
+      </c>
+      <c r="AE75">
+        <v>0.38</v>
       </c>
     </row>
     <row r="76" spans="1:31">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B76">
-        <v>0.24</v>
+        <v>0.44</v>
       </c>
       <c r="C76">
-        <v>0.64</v>
+        <v>0.31</v>
       </c>
       <c r="D76">
-        <v>0.12</v>
+        <v>0.26</v>
       </c>
       <c r="E76">
-        <v>0.55000000000000004</v>
+        <v>0.61</v>
       </c>
       <c r="F76">
-        <v>0.33</v>
+        <v>0.19</v>
       </c>
       <c r="G76">
         <v>0.08</v>
       </c>
       <c r="H76">
-        <v>0.04</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="77" spans="1:31">
       <c r="A77" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B77">
-        <v>0.28999999999999998</v>
+        <v>0.24</v>
       </c>
       <c r="C77">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="D77">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="E77">
-        <v>0.56999999999999995</v>
+        <v>0.48</v>
       </c>
       <c r="F77">
-        <v>0.31</v>
+        <v>0.35</v>
       </c>
       <c r="G77">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H77">
         <v>0.1</v>
@@ -3610,813 +3686,744 @@
     </row>
     <row r="78" spans="1:31">
       <c r="A78" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B78">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="C78">
-        <v>0.71</v>
+        <v>0.66</v>
       </c>
       <c r="D78">
+        <v>0.12</v>
+      </c>
+      <c r="E78">
+        <v>0.43</v>
+      </c>
+      <c r="F78">
+        <v>0.42</v>
+      </c>
+      <c r="G78">
+        <v>0.04</v>
+      </c>
+      <c r="H78">
         <v>0.1</v>
-      </c>
-      <c r="E78">
-        <v>0.48</v>
-      </c>
-      <c r="F78">
-        <v>0.38</v>
-      </c>
-      <c r="G78">
-        <v>0.09</v>
-      </c>
-      <c r="H78">
-        <v>0.05</v>
       </c>
     </row>
     <row r="79" spans="1:31">
       <c r="A79" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="B79">
-        <v>0.41</v>
+        <v>0.24</v>
       </c>
       <c r="C79">
-        <v>0.41</v>
+        <v>0.64</v>
       </c>
       <c r="D79">
-        <v>0.19</v>
+        <v>0.12</v>
       </c>
       <c r="E79">
-        <v>0.14000000000000001</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F79">
-        <v>0.46</v>
+        <v>0.33</v>
       </c>
       <c r="G79">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H79">
-        <v>0.31</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="80" spans="1:31">
       <c r="A80" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="B80">
-        <v>0.41</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C80">
-        <v>0.41</v>
+        <v>0.59</v>
       </c>
       <c r="D80">
-        <v>0.19</v>
+        <v>0.12</v>
       </c>
       <c r="E80">
-        <v>0.14000000000000001</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F80">
-        <v>0.46</v>
+        <v>0.31</v>
       </c>
       <c r="G80">
+        <v>0.03</v>
+      </c>
+      <c r="H80">
         <v>0.1</v>
-      </c>
-      <c r="H80">
-        <v>0.31</v>
       </c>
     </row>
     <row r="81" spans="1:31">
       <c r="A81" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="B81">
-        <v>0.49</v>
+        <v>0.19</v>
       </c>
       <c r="C81">
-        <v>0.35</v>
+        <v>0.71</v>
       </c>
       <c r="D81">
-        <v>0.16</v>
+        <v>0.1</v>
       </c>
       <c r="E81">
-        <v>0.04</v>
+        <v>0.48</v>
       </c>
       <c r="F81">
         <v>0.38</v>
       </c>
       <c r="G81">
-        <v>0.25</v>
+        <v>0.09</v>
       </c>
       <c r="H81">
-        <v>0.33</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="82" spans="1:31">
       <c r="A82" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B82">
-        <v>0.49</v>
+        <v>0.41</v>
       </c>
       <c r="C82">
-        <v>0.35</v>
+        <v>0.41</v>
       </c>
       <c r="D82">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="E82">
-        <v>0.04</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F82">
-        <v>0.38</v>
+        <v>0.46</v>
       </c>
       <c r="G82">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="H82">
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="83" spans="1:31">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="B83">
-        <v>0.17</v>
+        <v>0.41</v>
       </c>
       <c r="C83">
-        <v>0.65</v>
+        <v>0.41</v>
       </c>
       <c r="D83">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="E83">
-        <v>0.55000000000000004</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F83">
-        <v>0.28999999999999998</v>
+        <v>0.46</v>
       </c>
       <c r="G83">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="H83">
-        <v>0.09</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="84" spans="1:31">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="B84">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
       <c r="C84">
-        <v>0.18</v>
+        <v>0.35</v>
       </c>
       <c r="D84">
-        <v>0.32</v>
+        <v>0.16</v>
       </c>
       <c r="E84">
-        <v>0.19</v>
+        <v>0.04</v>
       </c>
       <c r="F84">
-        <v>0.34</v>
+        <v>0.38</v>
       </c>
       <c r="G84">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="H84">
-        <v>0.25</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="85" spans="1:31">
       <c r="A85" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="B85">
-        <v>0.1</v>
+        <v>0.49</v>
       </c>
       <c r="C85">
-        <v>0.88</v>
+        <v>0.35</v>
       </c>
       <c r="D85">
-        <v>0.03</v>
+        <v>0.16</v>
       </c>
       <c r="E85">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="F85">
-        <v>0.32</v>
+        <v>0.38</v>
       </c>
       <c r="G85">
-        <v>0.04</v>
+        <v>0.25</v>
       </c>
       <c r="H85">
-        <v>0.04</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="86" spans="1:31">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="B86">
-        <v>0.44</v>
+        <v>0.49</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="D86">
-        <v>0.56000000000000005</v>
+        <v>0.16</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H86">
-        <v>1</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="87" spans="1:31">
       <c r="A87" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="B87">
+        <v>0.17</v>
+      </c>
+      <c r="C87">
+        <v>0.65</v>
+      </c>
+      <c r="D87">
+        <v>0.18</v>
+      </c>
+      <c r="E87">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F87">
         <v>0.28999999999999998</v>
       </c>
-      <c r="C87">
-        <v>0.67</v>
-      </c>
-      <c r="D87">
-        <v>0.04</v>
-      </c>
-      <c r="E87">
-        <v>0.38</v>
-      </c>
-      <c r="F87">
-        <v>0.4</v>
-      </c>
       <c r="G87">
-        <v>0.13</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H87">
         <v>0.09</v>
       </c>
-      <c r="I87">
-        <v>2146</v>
-      </c>
-      <c r="J87">
-        <v>0.39</v>
-      </c>
-      <c r="K87">
-        <v>0.18</v>
-      </c>
-      <c r="L87">
-        <v>0.13</v>
-      </c>
-      <c r="M87">
-        <v>0.06</v>
-      </c>
-      <c r="N87">
-        <v>0.08</v>
-      </c>
-      <c r="O87">
-        <v>0.16</v>
-      </c>
-      <c r="P87">
-        <v>0.04</v>
-      </c>
-      <c r="Q87">
-        <v>0.16</v>
-      </c>
-      <c r="R87">
-        <v>0.13</v>
-      </c>
-      <c r="S87">
-        <v>0.54</v>
-      </c>
-      <c r="T87">
-        <v>0.1</v>
-      </c>
-      <c r="U87">
-        <v>0.03</v>
-      </c>
-      <c r="V87">
-        <v>0.03</v>
-      </c>
-      <c r="W87">
-        <v>0.12</v>
-      </c>
-      <c r="X87">
-        <v>0.09</v>
-      </c>
-      <c r="Y87">
-        <v>0.19</v>
-      </c>
-      <c r="Z87">
-        <v>0.31</v>
-      </c>
-      <c r="AA87">
-        <v>0.26</v>
-      </c>
-      <c r="AB87">
-        <v>0.02</v>
-      </c>
-      <c r="AC87">
-        <v>0.46</v>
-      </c>
-      <c r="AD87">
-        <v>0.36</v>
-      </c>
-      <c r="AE87">
-        <v>0.15</v>
-      </c>
     </row>
     <row r="88" spans="1:31">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B88">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C88">
-        <v>0.85</v>
+        <v>0.18</v>
       </c>
       <c r="D88">
-        <v>0.05</v>
+        <v>0.32</v>
       </c>
       <c r="E88">
-        <v>0.69</v>
+        <v>0.19</v>
       </c>
       <c r="F88">
-        <v>0.17</v>
+        <v>0.34</v>
       </c>
       <c r="G88">
-        <v>0.11</v>
+        <v>0.22</v>
       </c>
       <c r="H88">
-        <v>0.02</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="89" spans="1:31">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B89">
-        <v>0.17</v>
+        <v>0.1</v>
       </c>
       <c r="C89">
-        <v>0.78</v>
+        <v>0.88</v>
       </c>
       <c r="D89">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E89">
-        <v>0.53</v>
+        <v>0.59</v>
       </c>
       <c r="F89">
         <v>0.32</v>
       </c>
       <c r="G89">
-        <v>7.0000000000000007E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H89">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="90" spans="1:31">
       <c r="A90" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="B90">
-        <v>0.14000000000000001</v>
+        <v>0.44</v>
       </c>
       <c r="C90">
-        <v>0.86</v>
+        <v>0</v>
       </c>
       <c r="D90">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E90">
         <v>0</v>
       </c>
-      <c r="E90">
-        <v>0.36</v>
-      </c>
       <c r="F90">
-        <v>0.32</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>0.27</v>
+        <v>0</v>
       </c>
       <c r="H90">
-        <v>0.04</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:31">
       <c r="A91" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="B91">
-        <v>0.14000000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C91">
-        <v>0.86</v>
+        <v>0.67</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="E91">
+        <v>0.38</v>
+      </c>
+      <c r="F91">
+        <v>0.4</v>
+      </c>
+      <c r="G91">
+        <v>0.13</v>
+      </c>
+      <c r="H91">
+        <v>0.09</v>
+      </c>
+      <c r="I91">
+        <v>2146</v>
+      </c>
+      <c r="J91">
+        <v>0.39</v>
+      </c>
+      <c r="K91">
+        <v>0.18</v>
+      </c>
+      <c r="L91">
+        <v>0.13</v>
+      </c>
+      <c r="M91">
+        <v>0.06</v>
+      </c>
+      <c r="N91">
+        <v>0.08</v>
+      </c>
+      <c r="O91">
+        <v>0.16</v>
+      </c>
+      <c r="P91">
+        <v>0.04</v>
+      </c>
+      <c r="Q91">
+        <v>0.16</v>
+      </c>
+      <c r="R91">
+        <v>0.13</v>
+      </c>
+      <c r="S91">
+        <v>0.54</v>
+      </c>
+      <c r="T91">
+        <v>0.1</v>
+      </c>
+      <c r="U91">
+        <v>0.03</v>
+      </c>
+      <c r="V91">
+        <v>0.03</v>
+      </c>
+      <c r="W91">
+        <v>0.12</v>
+      </c>
+      <c r="X91">
+        <v>0.09</v>
+      </c>
+      <c r="Y91">
+        <v>0.19</v>
+      </c>
+      <c r="Z91">
+        <v>0.31</v>
+      </c>
+      <c r="AA91">
+        <v>0.26</v>
+      </c>
+      <c r="AB91">
+        <v>0.02</v>
+      </c>
+      <c r="AC91">
+        <v>0.46</v>
+      </c>
+      <c r="AD91">
         <v>0.36</v>
       </c>
-      <c r="F91">
-        <v>0.32</v>
-      </c>
-      <c r="G91">
-        <v>0.27</v>
-      </c>
-      <c r="H91">
-        <v>0.04</v>
+      <c r="AE91">
+        <v>0.15</v>
       </c>
     </row>
     <row r="92" spans="1:31">
       <c r="A92" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="B92">
-        <v>0.87</v>
+        <v>0.1</v>
       </c>
       <c r="C92">
-        <v>0.03</v>
+        <v>0.85</v>
       </c>
       <c r="D92">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E92">
-        <v>0.55000000000000004</v>
+        <v>0.69</v>
       </c>
       <c r="F92">
-        <v>0.3</v>
+        <v>0.17</v>
       </c>
       <c r="G92">
-        <v>0.15</v>
+        <v>0.11</v>
       </c>
       <c r="H92">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="93" spans="1:31">
       <c r="A93" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B93">
-        <v>0.27</v>
+        <v>0.17</v>
       </c>
       <c r="C93">
-        <v>0.73</v>
+        <v>0.78</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E93">
-        <v>0.37</v>
+        <v>0.53</v>
       </c>
       <c r="F93">
-        <v>0.46</v>
+        <v>0.32</v>
       </c>
       <c r="G93">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H93">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="94" spans="1:31">
       <c r="A94" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B94">
-        <v>0.48</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C94">
-        <v>0.5</v>
+        <v>0.86</v>
       </c>
       <c r="D94">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="E94">
-        <v>0.12</v>
+        <v>0.36</v>
       </c>
       <c r="F94">
-        <v>0.55000000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="G94">
-        <v>0.18</v>
+        <v>0.27</v>
       </c>
       <c r="H94">
-        <v>0.14000000000000001</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="95" spans="1:31">
       <c r="A95" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B95">
-        <v>0.48</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C95">
-        <v>0.5</v>
+        <v>0.86</v>
       </c>
       <c r="D95">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="E95">
-        <v>0.12</v>
+        <v>0.36</v>
       </c>
       <c r="F95">
-        <v>0.55000000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="G95">
-        <v>0.18</v>
+        <v>0.27</v>
       </c>
       <c r="H95">
-        <v>0.14000000000000001</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="96" spans="1:31">
       <c r="A96" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="B96">
-        <v>0.31</v>
+        <v>0.87</v>
       </c>
       <c r="C96">
-        <v>0.64</v>
+        <v>0.03</v>
       </c>
       <c r="D96">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E96">
-        <v>0.32</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F96">
-        <v>0.43</v>
+        <v>0.3</v>
       </c>
       <c r="G96">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="H96">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:31">
       <c r="A97" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B97">
-        <v>0.31</v>
+        <v>0.27</v>
       </c>
       <c r="C97">
-        <v>0.64</v>
+        <v>0.73</v>
       </c>
       <c r="D97">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E97">
-        <v>0.22</v>
+        <v>0.37</v>
       </c>
       <c r="F97">
-        <v>0.53</v>
+        <v>0.46</v>
       </c>
       <c r="G97">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H97">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="98" spans="1:31">
       <c r="A98" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B98">
-        <v>0.28000000000000003</v>
+        <v>0.48</v>
       </c>
       <c r="C98">
-        <v>0.67</v>
+        <v>0.5</v>
       </c>
       <c r="D98">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="E98">
-        <v>0.32</v>
+        <v>0.12</v>
       </c>
       <c r="F98">
-        <v>0.48</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G98">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
       <c r="H98">
-        <v>0.11</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="99" spans="1:31">
       <c r="A99" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B99">
-        <v>0.28000000000000003</v>
+        <v>0.48</v>
       </c>
       <c r="C99">
-        <v>0.67</v>
+        <v>0.5</v>
       </c>
       <c r="D99">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="E99">
-        <v>0.32</v>
+        <v>0.12</v>
       </c>
       <c r="F99">
-        <v>0.48</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G99">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
       <c r="H99">
-        <v>0.11</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="100" spans="1:31">
       <c r="A100" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="B100">
-        <v>0.87</v>
+        <v>0.31</v>
       </c>
       <c r="C100">
-        <v>0.03</v>
+        <v>0.64</v>
       </c>
       <c r="D100">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E100">
-        <v>0.55000000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="F100">
-        <v>0.3</v>
+        <v>0.43</v>
       </c>
       <c r="G100">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="H100">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="101" spans="1:31">
       <c r="A101" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="B101">
-        <v>0.87</v>
+        <v>0.31</v>
       </c>
       <c r="C101">
-        <v>0.03</v>
+        <v>0.64</v>
       </c>
       <c r="D101">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E101">
-        <v>0.55000000000000004</v>
+        <v>0.22</v>
       </c>
       <c r="F101">
-        <v>0.3</v>
+        <v>0.53</v>
       </c>
       <c r="G101">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="H101">
-        <v>0</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="102" spans="1:31">
       <c r="A102" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="B102">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C102">
-        <v>0.61</v>
+        <v>0.67</v>
       </c>
       <c r="D102">
+        <v>0.05</v>
+      </c>
+      <c r="E102">
+        <v>0.32</v>
+      </c>
+      <c r="F102">
+        <v>0.48</v>
+      </c>
+      <c r="G102">
         <v>0.09</v>
       </c>
-      <c r="E102">
-        <v>0.26</v>
-      </c>
-      <c r="F102">
-        <v>0.46</v>
-      </c>
-      <c r="G102">
-        <v>0.18</v>
-      </c>
       <c r="H102">
-        <v>0.1</v>
-      </c>
-      <c r="I102">
-        <v>2014</v>
-      </c>
-      <c r="J102">
-        <v>0.44</v>
-      </c>
-      <c r="K102">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="L102">
-        <v>0.15</v>
-      </c>
-      <c r="M102">
-        <v>0.04</v>
-      </c>
-      <c r="N102">
-        <v>0.09</v>
-      </c>
-      <c r="O102">
-        <v>0.13</v>
-      </c>
-      <c r="P102">
-        <v>0.04</v>
-      </c>
-      <c r="Q102">
-        <v>0.21</v>
-      </c>
-      <c r="R102">
-        <v>0.1</v>
-      </c>
-      <c r="S102">
-        <v>0.52</v>
-      </c>
-      <c r="T102">
-        <v>0.08</v>
-      </c>
-      <c r="U102">
-        <v>0.03</v>
-      </c>
-      <c r="V102">
-        <v>0.05</v>
-      </c>
-      <c r="W102">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="X102">
-        <v>0.09</v>
-      </c>
-      <c r="Y102">
-        <v>0.21</v>
-      </c>
-      <c r="Z102">
-        <v>0.31</v>
-      </c>
-      <c r="AA102">
-        <v>0.21</v>
-      </c>
-      <c r="AB102">
-        <v>0.03</v>
-      </c>
-      <c r="AC102">
-        <v>0.43</v>
-      </c>
-      <c r="AD102">
-        <v>0.4</v>
-      </c>
-      <c r="AE102">
-        <v>0.14000000000000001</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="103" spans="1:31">
       <c r="A103" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B103">
-        <v>0.23</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C103">
-        <v>0.7</v>
+        <v>0.67</v>
       </c>
       <c r="D103">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E103">
-        <v>0.18</v>
+        <v>0.32</v>
       </c>
       <c r="F103">
-        <v>0.53</v>
+        <v>0.48</v>
       </c>
       <c r="G103">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="H103">
         <v>0.11</v>
@@ -4424,370 +4431,569 @@
     </row>
     <row r="104" spans="1:31">
       <c r="A104" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B104">
-        <f>AVERAGE(B105:B106)</f>
-        <v>0.245</v>
+        <v>0.87</v>
       </c>
       <c r="C104">
-        <f>AVERAGE(C105:C106)</f>
-        <v>0.71499999999999997</v>
+        <v>0.03</v>
       </c>
       <c r="D104">
-        <f>AVERAGE(D105:D106)</f>
-        <v>4.4999999999999998E-2</v>
+        <v>0.1</v>
       </c>
       <c r="E104">
-        <f>AVERAGE(E105:E106)</f>
-        <v>0.30499999999999999</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F104">
-        <f>AVERAGE(F105:F106)</f>
-        <v>0.505</v>
+        <v>0.3</v>
       </c>
       <c r="G104">
-        <f>AVERAGE(G105:G106)</f>
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
       <c r="H104">
-        <f>AVERAGE(H105:H106)</f>
-        <v>6.5000000000000002E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:31">
       <c r="A105" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="B105">
-        <v>0.25</v>
+        <v>0.87</v>
       </c>
       <c r="C105">
-        <v>0.71</v>
+        <v>0.03</v>
       </c>
       <c r="D105">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E105">
-        <v>0.39</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F105">
-        <v>0.49</v>
+        <v>0.3</v>
       </c>
       <c r="G105">
-        <v>0.09</v>
+        <v>0.15</v>
       </c>
       <c r="H105">
-        <v>0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:31">
       <c r="A106" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="B106">
-        <v>0.24</v>
+        <v>0.31</v>
       </c>
       <c r="C106">
-        <v>0.72</v>
+        <v>0.64</v>
       </c>
       <c r="D106">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E106">
         <v>0.22</v>
       </c>
       <c r="F106">
-        <v>0.52</v>
+        <v>0.53</v>
       </c>
       <c r="G106">
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
       <c r="H106">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="107" spans="1:31">
       <c r="A107" t="s">
-        <v>143</v>
+        <v>7</v>
       </c>
       <c r="B107">
-        <f>AVERAGE(B108:B109)</f>
-        <v>0.42499999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="C107">
-        <f>AVERAGE(C108:C109)</f>
-        <v>0.47500000000000003</v>
+        <v>0.61</v>
       </c>
       <c r="D107">
-        <f>AVERAGE(D108:D109)</f>
+        <v>0.09</v>
+      </c>
+      <c r="E107">
+        <v>0.26</v>
+      </c>
+      <c r="F107">
+        <v>0.46</v>
+      </c>
+      <c r="G107">
+        <v>0.18</v>
+      </c>
+      <c r="H107">
         <v>0.1</v>
       </c>
-      <c r="E107">
-        <f>AVERAGE(E108:E109)</f>
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="F107">
-        <f>AVERAGE(F108:F109)</f>
-        <v>0.24000000000000002</v>
-      </c>
-      <c r="G107">
-        <f>AVERAGE(G108:G109)</f>
-        <v>0.19</v>
-      </c>
-      <c r="H107">
-        <f>AVERAGE(H108:H109)</f>
-        <v>7.4999999999999997E-2</v>
+      <c r="I107">
+        <v>2014</v>
+      </c>
+      <c r="J107">
+        <v>0.44</v>
+      </c>
+      <c r="K107">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L107">
+        <v>0.15</v>
+      </c>
+      <c r="M107">
+        <v>0.04</v>
+      </c>
+      <c r="N107">
+        <v>0.09</v>
+      </c>
+      <c r="O107">
+        <v>0.13</v>
+      </c>
+      <c r="P107">
+        <v>0.04</v>
+      </c>
+      <c r="Q107">
+        <v>0.21</v>
+      </c>
+      <c r="R107">
+        <v>0.1</v>
+      </c>
+      <c r="S107">
+        <v>0.52</v>
+      </c>
+      <c r="T107">
+        <v>0.08</v>
+      </c>
+      <c r="U107">
+        <v>0.03</v>
+      </c>
+      <c r="V107">
+        <v>0.05</v>
+      </c>
+      <c r="W107">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="X107">
+        <v>0.09</v>
+      </c>
+      <c r="Y107">
+        <v>0.21</v>
+      </c>
+      <c r="Z107">
+        <v>0.31</v>
+      </c>
+      <c r="AA107">
+        <v>0.21</v>
+      </c>
+      <c r="AB107">
+        <v>0.03</v>
+      </c>
+      <c r="AC107">
+        <v>0.43</v>
+      </c>
+      <c r="AD107">
+        <v>0.4</v>
+      </c>
+      <c r="AE107">
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="108" spans="1:31">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
       <c r="B108">
-        <v>0.6</v>
+        <v>0.23</v>
       </c>
       <c r="C108">
-        <v>0.27</v>
+        <v>0.7</v>
       </c>
       <c r="D108">
-        <v>0.13</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E108">
-        <v>0.72</v>
+        <v>0.18</v>
       </c>
       <c r="F108">
-        <v>0.02</v>
+        <v>0.53</v>
       </c>
       <c r="G108">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
       <c r="H108">
-        <v>0.04</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="109" spans="1:31">
       <c r="A109" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="B109">
-        <v>0.25</v>
+        <f>AVERAGE(B110:B111)</f>
+        <v>0.245</v>
       </c>
       <c r="C109">
-        <v>0.68</v>
+        <f>AVERAGE(C110:C111)</f>
+        <v>0.71499999999999997</v>
       </c>
       <c r="D109">
-        <v>7.0000000000000007E-2</v>
+        <f>AVERAGE(D110:D111)</f>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E109">
-        <v>0.25</v>
+        <f>AVERAGE(E110:E111)</f>
+        <v>0.30499999999999999</v>
       </c>
       <c r="F109">
-        <v>0.46</v>
+        <f>AVERAGE(F110:F111)</f>
+        <v>0.505</v>
       </c>
       <c r="G109">
-        <v>0.17</v>
+        <f>AVERAGE(G110:G111)</f>
+        <v>0.125</v>
       </c>
       <c r="H109">
-        <v>0.11</v>
+        <f>AVERAGE(H110:H111)</f>
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="110" spans="1:31">
       <c r="A110" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B110">
-        <v>0.45</v>
+        <v>0.25</v>
       </c>
       <c r="C110">
-        <v>0.22</v>
+        <v>0.71</v>
       </c>
       <c r="D110">
-        <v>0.34</v>
+        <v>0.05</v>
       </c>
       <c r="E110">
-        <v>0.16</v>
+        <v>0.39</v>
       </c>
       <c r="F110">
-        <v>0.38</v>
+        <v>0.49</v>
       </c>
       <c r="G110">
-        <v>0.24</v>
+        <v>0.09</v>
       </c>
       <c r="H110">
-        <v>0.23</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="111" spans="1:31">
       <c r="A111" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="B111">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="C111">
-        <v>0.7</v>
+        <v>0.72</v>
       </c>
       <c r="D111">
-        <v>7.0000000000000007E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E111">
-        <v>0.18</v>
+        <v>0.22</v>
       </c>
       <c r="F111">
-        <v>0.53</v>
+        <v>0.52</v>
       </c>
       <c r="G111">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="H111">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="112" spans="1:31">
       <c r="A112" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="B112">
-        <v>0.37</v>
+        <f>AVERAGE(B113:B114)</f>
+        <v>0.42499999999999999</v>
       </c>
       <c r="C112">
-        <v>0.5</v>
+        <f>AVERAGE(C113:C114)</f>
+        <v>0.47500000000000003</v>
       </c>
       <c r="D112">
-        <v>0.13</v>
+        <f>AVERAGE(D113:D114)</f>
+        <v>0.1</v>
       </c>
       <c r="E112">
-        <v>0.25</v>
+        <f>AVERAGE(E113:E114)</f>
+        <v>0.48499999999999999</v>
       </c>
       <c r="F112">
-        <v>0.35</v>
+        <f>AVERAGE(F113:F114)</f>
+        <v>0.24000000000000002</v>
       </c>
       <c r="G112">
-        <v>0.27</v>
+        <f>AVERAGE(G113:G114)</f>
+        <v>0.19</v>
       </c>
       <c r="H112">
-        <v>0.12</v>
+        <f>AVERAGE(H113:H114)</f>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="113" spans="1:31">
       <c r="A113" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B113">
-        <v>0.52</v>
+        <v>0.6</v>
       </c>
       <c r="C113">
-        <v>0.42</v>
+        <v>0.27</v>
       </c>
       <c r="D113">
-        <v>0.06</v>
+        <v>0.13</v>
       </c>
       <c r="E113">
-        <v>0.46</v>
+        <v>0.72</v>
       </c>
       <c r="F113">
-        <v>0.31</v>
+        <v>0.02</v>
       </c>
       <c r="G113">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="H113">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="114" spans="1:31">
       <c r="A114" t="s">
+        <v>103</v>
+      </c>
+      <c r="B114">
+        <v>0.25</v>
+      </c>
+      <c r="C114">
+        <v>0.68</v>
+      </c>
+      <c r="D114">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E114">
+        <v>0.25</v>
+      </c>
+      <c r="F114">
+        <v>0.46</v>
+      </c>
+      <c r="G114">
+        <v>0.17</v>
+      </c>
+      <c r="H114">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:31">
+      <c r="A115" t="s">
+        <v>104</v>
+      </c>
+      <c r="B115">
+        <v>0.45</v>
+      </c>
+      <c r="C115">
+        <v>0.22</v>
+      </c>
+      <c r="D115">
+        <v>0.34</v>
+      </c>
+      <c r="E115">
+        <v>0.16</v>
+      </c>
+      <c r="F115">
+        <v>0.38</v>
+      </c>
+      <c r="G115">
+        <v>0.24</v>
+      </c>
+      <c r="H115">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="116" spans="1:31">
+      <c r="A116" t="s">
+        <v>138</v>
+      </c>
+      <c r="B116">
+        <v>0.23</v>
+      </c>
+      <c r="C116">
+        <v>0.7</v>
+      </c>
+      <c r="D116">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E116">
+        <v>0.18</v>
+      </c>
+      <c r="F116">
+        <v>0.53</v>
+      </c>
+      <c r="G116">
+        <v>0.18</v>
+      </c>
+      <c r="H116">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="117" spans="1:31">
+      <c r="A117" t="s">
+        <v>105</v>
+      </c>
+      <c r="B117">
+        <v>0.37</v>
+      </c>
+      <c r="C117">
+        <v>0.5</v>
+      </c>
+      <c r="D117">
+        <v>0.13</v>
+      </c>
+      <c r="E117">
+        <v>0.25</v>
+      </c>
+      <c r="F117">
+        <v>0.35</v>
+      </c>
+      <c r="G117">
+        <v>0.27</v>
+      </c>
+      <c r="H117">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="118" spans="1:31">
+      <c r="A118" t="s">
+        <v>106</v>
+      </c>
+      <c r="B118">
+        <v>0.52</v>
+      </c>
+      <c r="C118">
+        <v>0.42</v>
+      </c>
+      <c r="D118">
+        <v>0.06</v>
+      </c>
+      <c r="E118">
+        <v>0.46</v>
+      </c>
+      <c r="F118">
+        <v>0.31</v>
+      </c>
+      <c r="G118">
+        <v>0.24</v>
+      </c>
+      <c r="H118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:31">
+      <c r="A119" t="s">
         <v>38</v>
       </c>
-      <c r="B114">
+      <c r="B119">
         <v>0.32</v>
       </c>
-      <c r="C114">
+      <c r="C119">
         <v>0.46</v>
       </c>
-      <c r="D114">
+      <c r="D119">
         <v>0.22</v>
       </c>
-      <c r="E114">
+      <c r="E119">
         <v>0.41</v>
       </c>
-      <c r="F114">
+      <c r="F119">
         <v>0.33</v>
       </c>
-      <c r="G114">
+      <c r="G119">
         <v>0.11</v>
       </c>
-      <c r="H114">
+      <c r="H119">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I114">
+      <c r="I119">
         <v>2489</v>
       </c>
-      <c r="J114">
+      <c r="J119">
         <v>0.32</v>
       </c>
-      <c r="K114">
+      <c r="K119">
         <v>0.16</v>
       </c>
-      <c r="L114">
+      <c r="L119">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M114">
+      <c r="M119">
         <v>0.06</v>
       </c>
-      <c r="N114">
+      <c r="N119">
         <v>0.09</v>
       </c>
-      <c r="O114">
+      <c r="O119">
         <v>0.23</v>
       </c>
-      <c r="P114">
+      <c r="P119">
         <v>0.1</v>
       </c>
-      <c r="Q114">
+      <c r="Q119">
         <v>0.16</v>
       </c>
-      <c r="R114">
+      <c r="R119">
         <v>0.22</v>
       </c>
-      <c r="S114">
+      <c r="S119">
         <v>0.35</v>
       </c>
-      <c r="T114">
+      <c r="T119">
         <v>0.13</v>
       </c>
-      <c r="U114">
+      <c r="U119">
         <v>0.05</v>
       </c>
-      <c r="V114">
+      <c r="V119">
         <v>0.06</v>
       </c>
-      <c r="W114">
+      <c r="W119">
         <v>0.18</v>
       </c>
-      <c r="X114">
+      <c r="X119">
         <v>0.11</v>
       </c>
-      <c r="Y114">
+      <c r="Y119">
         <v>0.18</v>
       </c>
-      <c r="Z114">
+      <c r="Z119">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AA114">
+      <c r="AA119">
         <v>0.19</v>
       </c>
-      <c r="AB114">
+      <c r="AB119">
         <v>0.03</v>
       </c>
-      <c r="AC114">
+      <c r="AC119">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AD114">
+      <c r="AD119">
         <v>0.33</v>
       </c>
-      <c r="AE114">
+      <c r="AE119">
         <v>0.35</v>
       </c>
     </row>

</xml_diff>